<commit_message>
Adding conceptual integrated model for testing integration methods.
</commit_message>
<xml_diff>
--- a/tests/integration/models/5 - coupled_model/sets.xlsx
+++ b/tests/integration/models/5 - coupled_model/sets.xlsx
@@ -8,98 +8,71 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\5 - coupled_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E02A0F-9EA3-4227-8602-A98D236C6DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CE75E9-B8A7-4AE9-8D56-FD099F681997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17650" yWindow="3420" windowWidth="13410" windowHeight="15370" tabRatio="944" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="_set_TECHNOLOGIES" sheetId="1" r:id="rId1"/>
-    <sheet name="_set_PRODUCTS" sheetId="2" r:id="rId2"/>
-    <sheet name="_set_AIR_EMISSIONS" sheetId="3" r:id="rId3"/>
+    <sheet name="_set_PRODUCTS" sheetId="1" r:id="rId1"/>
+    <sheet name="_set_PRODUCT_DATA" sheetId="2" r:id="rId2"/>
+    <sheet name="_set_RESOURCES" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
-  <si>
-    <t>t_Names</t>
-  </si>
-  <si>
-    <t>t_Mix</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>p_Names</t>
   </si>
   <si>
-    <t>p_Mix</t>
-  </si>
-  <si>
-    <t>e_Names</t>
-  </si>
-  <si>
-    <t>air emissions</t>
-  </si>
-  <si>
-    <t>heat</t>
-  </si>
-  <si>
-    <t>electricity chp</t>
-  </si>
-  <si>
-    <t>electricity pv</t>
-  </si>
-  <si>
-    <t>fuel A</t>
-  </si>
-  <si>
-    <t>fuel B</t>
-  </si>
-  <si>
-    <t>product A</t>
-  </si>
-  <si>
-    <t>product B</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>boiler</t>
-  </si>
-  <si>
-    <t>chp engine</t>
-  </si>
-  <si>
-    <t>pv plant</t>
-  </si>
-  <si>
-    <t>oil refinery</t>
-  </si>
-  <si>
-    <t>industry</t>
-  </si>
-  <si>
-    <t>p_Assumption</t>
-  </si>
-  <si>
-    <t>product-technology</t>
-  </si>
-  <si>
-    <t>industry-technology</t>
-  </si>
-  <si>
-    <t>t_Assumption</t>
+    <t>pd_Names</t>
+  </si>
+  <si>
+    <t>pd_Category</t>
+  </si>
+  <si>
+    <t>r_Names</t>
+  </si>
+  <si>
+    <t>product 1</t>
+  </si>
+  <si>
+    <t>product 2</t>
+  </si>
+  <si>
+    <t>energy_use</t>
+  </si>
+  <si>
+    <t>unit profit</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>energy availability</t>
+  </si>
+  <si>
+    <t>unit energy use, initial</t>
+  </si>
+  <si>
+    <t>unit energy use</t>
+  </si>
+  <si>
+    <t>energy_use_0</t>
+  </si>
+  <si>
+    <t>learning rate</t>
+  </si>
+  <si>
+    <t>learning_rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0;\-0;\-"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,6 +85,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,12 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,185 +430,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>